<commit_message>
Add randomness and bug fixes
</commit_message>
<xml_diff>
--- a/old.xlsx
+++ b/old.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andybenichou/Desktop/meshavsek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BF61C2-A49C-574B-B1FB-293F5B994C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A34F63-2777-1B4B-9DE0-E04D5E9342BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -438,14 +438,28 @@
     <xf numFmtId="20" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -459,40 +473,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -506,10 +488,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -733,10 +733,10 @@
   <dimension ref="A1:Y982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H37" sqref="H37"/>
+      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -792,25 +792,25 @@
       <c r="Y1" s="4"/>
     </row>
     <row r="2" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="5">
         <v>1.0833333333333333</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="4"/>
@@ -833,15 +833,15 @@
       <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="6">
         <v>1.125</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -862,15 +862,15 @@
       <c r="Y3" s="4"/>
     </row>
     <row r="4" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="5">
         <v>1.1666666666666667</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="15"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="11"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -891,23 +891,23 @@
       <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="6">
         <v>1.2083333333333333</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="16"/>
+      <c r="G5" s="12"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -928,15 +928,15 @@
       <c r="Y5" s="4"/>
     </row>
     <row r="6" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="5">
         <v>1.25</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="22"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -957,15 +957,15 @@
       <c r="Y6" s="4"/>
     </row>
     <row r="7" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="6">
         <v>1.2916666666666667</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -986,21 +986,21 @@
       <c r="Y7" s="4"/>
     </row>
     <row r="8" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="7">
         <v>1.3333333333333333</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="15"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1021,15 +1021,15 @@
       <c r="Y8" s="4"/>
     </row>
     <row r="9" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="6">
         <v>1.375</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="15"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -1050,15 +1050,15 @@
       <c r="Y9" s="4"/>
     </row>
     <row r="10" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="5">
         <v>1.4166666666666667</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="15"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1079,21 +1079,21 @@
       <c r="Y10" s="4"/>
     </row>
     <row r="11" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="6">
         <v>1.4583333333333333</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="15"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -1114,15 +1114,15 @@
       <c r="Y11" s="4"/>
     </row>
     <row r="12" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="5">
         <v>1.5</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="15"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1143,15 +1143,15 @@
       <c r="Y12" s="4"/>
     </row>
     <row r="13" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="6">
         <v>1.5416666666666667</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="15"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="11"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -1172,21 +1172,21 @@
       <c r="Y13" s="4"/>
     </row>
     <row r="14" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="5">
         <v>1.5833333333333333</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="15"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1207,15 +1207,15 @@
       <c r="Y14" s="4"/>
     </row>
     <row r="15" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="6">
         <v>1.625</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="15"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -1236,15 +1236,15 @@
       <c r="Y15" s="4"/>
     </row>
     <row r="16" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="5">
         <v>1.6666666666666667</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="15"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -1265,21 +1265,21 @@
       <c r="Y16" s="4"/>
     </row>
     <row r="17" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="6">
         <v>1.7083333333333333</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="15"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="11"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1300,15 +1300,15 @@
       <c r="Y17" s="4"/>
     </row>
     <row r="18" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="5">
         <v>1.75</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="15"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -1329,15 +1329,15 @@
       <c r="Y18" s="4"/>
     </row>
     <row r="19" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="6">
         <v>1.7916666666666667</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="16"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -1358,23 +1358,23 @@
       <c r="Y19" s="4"/>
     </row>
     <row r="20" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="5">
         <v>1.8333333333333333</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="24"/>
+      <c r="G20" s="32"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -1395,15 +1395,15 @@
       <c r="Y20" s="4"/>
     </row>
     <row r="21" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="6">
         <v>1.875</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="12"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -1424,15 +1424,15 @@
       <c r="Y21" s="4"/>
     </row>
     <row r="22" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="5">
         <v>1.9166666666666667</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="14" t="s">
+      <c r="C22" s="12"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="4"/>
@@ -1455,23 +1455,23 @@
       <c r="Y22" s="4"/>
     </row>
     <row r="23" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="6">
         <v>1.9583333333333333</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="15"/>
+      <c r="G23" s="11"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1492,17 +1492,17 @@
       <c r="Y23" s="4"/>
     </row>
     <row r="24" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -1523,15 +1523,15 @@
       <c r="Y24" s="4"/>
     </row>
     <row r="25" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="6">
         <v>1.0416666666666667</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -1552,23 +1552,23 @@
       <c r="Y25" s="4"/>
     </row>
     <row r="26" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="5">
         <v>1.0833333333333333</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="21" t="s">
         <v>24</v>
       </c>
       <c r="H26" s="4"/>
@@ -1591,15 +1591,15 @@
       <c r="Y26" s="4"/>
     </row>
     <row r="27" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="6">
         <v>1.125</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1620,15 +1620,15 @@
       <c r="Y27" s="4"/>
     </row>
     <row r="28" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="5">
         <v>1.1666666666666667</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="15"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -1649,23 +1649,23 @@
       <c r="Y28" s="4"/>
     </row>
     <row r="29" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="6">
         <v>1.2083333333333333</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G29" s="16"/>
+      <c r="G29" s="12"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -1686,15 +1686,15 @@
       <c r="Y29" s="4"/>
     </row>
     <row r="30" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="5">
         <v>1.25</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="22"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="10"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -1715,15 +1715,15 @@
       <c r="Y30" s="4"/>
     </row>
     <row r="31" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="6">
         <v>1.2916666666666667</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -1744,21 +1744,21 @@
       <c r="Y31" s="4"/>
     </row>
     <row r="32" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="7">
         <v>1.3333333333333333</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
@@ -1779,15 +1779,15 @@
       <c r="Y32" s="4"/>
     </row>
     <row r="33" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="6">
         <v>1.375</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="15"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="11"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -1808,15 +1808,15 @@
       <c r="Y33" s="4"/>
     </row>
     <row r="34" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="5">
         <v>1.4166666666666667</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="15"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="11"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -1837,21 +1837,21 @@
       <c r="Y34" s="4"/>
     </row>
     <row r="35" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="6">
         <v>1.4583333333333333</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F35" s="30"/>
-      <c r="G35" s="15"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="11"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -1872,15 +1872,15 @@
       <c r="Y35" s="4"/>
     </row>
     <row r="36" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="5">
         <v>1.5</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="15"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="11"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -1901,15 +1901,15 @@
       <c r="Y36" s="4"/>
     </row>
     <row r="37" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="6">
         <v>1.5416666666666667</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="15"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -1930,21 +1930,21 @@
       <c r="Y37" s="4"/>
     </row>
     <row r="38" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="5">
         <v>1.5833333333333333</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F38" s="30"/>
-      <c r="G38" s="15"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="11"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -1965,15 +1965,15 @@
       <c r="Y38" s="4"/>
     </row>
     <row r="39" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="8"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="6">
         <v>1.625</v>
       </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="15"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="11"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -1994,15 +1994,15 @@
       <c r="Y39" s="4"/>
     </row>
     <row r="40" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="5">
         <v>1.6666666666666667</v>
       </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="15"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="11"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -2023,21 +2023,21 @@
       <c r="Y40" s="4"/>
     </row>
     <row r="41" spans="1:25" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="6">
         <v>1.7083333333333333</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="30"/>
-      <c r="G41" s="15"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="11"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -2058,15 +2058,15 @@
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="5">
         <v>1.75</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="15"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="11"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -2087,15 +2087,15 @@
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="6">
         <v>1.7916666666666667</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="16"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="12"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
@@ -2116,15 +2116,15 @@
       <c r="Y43" s="4"/>
     </row>
     <row r="44" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="5">
         <v>1.8333333333333333</v>
       </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="32"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="26"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -2145,15 +2145,15 @@
       <c r="Y44" s="4"/>
     </row>
     <row r="45" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="6">
         <v>1.875</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="16"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="12"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -2174,15 +2174,15 @@
       <c r="Y45" s="4"/>
     </row>
     <row r="46" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="5">
         <v>1.9166666666666667</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="21"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="28"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
@@ -2203,15 +2203,15 @@
       <c r="Y46" s="4"/>
     </row>
     <row r="47" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="6">
         <v>1.9583333333333333</v>
       </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="15"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="11"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -2232,17 +2232,17 @@
       <c r="Y47" s="4"/>
     </row>
     <row r="48" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="34" t="s">
         <v>41</v>
       </c>
       <c r="B48" s="5">
         <v>1</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
@@ -2263,15 +2263,15 @@
       <c r="Y48" s="4"/>
     </row>
     <row r="49" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="9"/>
+      <c r="A49" s="34"/>
       <c r="B49" s="6">
         <v>1.0416666666666667</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
@@ -2292,15 +2292,15 @@
       <c r="Y49" s="4"/>
     </row>
     <row r="50" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="9"/>
+      <c r="A50" s="34"/>
       <c r="B50" s="5">
         <v>1.0833333333333333</v>
       </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
@@ -2321,15 +2321,15 @@
       <c r="Y50" s="4"/>
     </row>
     <row r="51" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="9"/>
+      <c r="A51" s="34"/>
       <c r="B51" s="6">
         <v>1.125</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
@@ -2350,15 +2350,15 @@
       <c r="Y51" s="4"/>
     </row>
     <row r="52" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="9"/>
+      <c r="A52" s="34"/>
       <c r="B52" s="5">
         <v>1.1666666666666667</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="15"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="11"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
@@ -2379,15 +2379,15 @@
       <c r="Y52" s="4"/>
     </row>
     <row r="53" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="9"/>
+      <c r="A53" s="34"/>
       <c r="B53" s="6">
         <v>1.2083333333333333</v>
       </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="16"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="12"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
@@ -2408,15 +2408,15 @@
       <c r="Y53" s="4"/>
     </row>
     <row r="54" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="9"/>
+      <c r="A54" s="34"/>
       <c r="B54" s="5">
         <v>1.25</v>
       </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="22"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="10"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
@@ -2437,15 +2437,15 @@
       <c r="Y54" s="4"/>
     </row>
     <row r="55" spans="1:25" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="10"/>
+      <c r="A55" s="35"/>
       <c r="B55" s="6">
         <v>1.2916666666666667</v>
       </c>
-      <c r="C55" s="16"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
@@ -27496,6 +27496,69 @@
     </row>
   </sheetData>
   <mergeCells count="79">
+    <mergeCell ref="A24:A47"/>
+    <mergeCell ref="A48:A55"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="G46:G49"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="F32:G43"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="F8:G19"/>
     <mergeCell ref="A2:A23"/>
     <mergeCell ref="G50:G53"/>
     <mergeCell ref="G54:G55"/>
@@ -27512,69 +27575,6 @@
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="F32:G43"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="F8:G19"/>
-    <mergeCell ref="G46:G49"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="A24:A47"/>
-    <mergeCell ref="A48:A55"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="E53:E55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>